<commit_message>
commit-added Spring 2019 degree plan with summer and without summer
</commit_message>
<xml_diff>
--- a/DegreeAudit.xlsx
+++ b/DegreeAudit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="4545" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="5" r:id="rId1"/>
@@ -1882,8 +1882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2194,8 +2194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2204,7 +2204,7 @@
     <col min="3" max="3" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2490,6 +2490,7 @@
       <c r="E15" s="4" t="s">
         <v>53</v>
       </c>
+      <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
@@ -2507,8 +2508,9 @@
       <c r="E16" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2524,8 +2526,9 @@
       <c r="E17" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -2541,8 +2544,9 @@
       <c r="E18" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -2558,8 +2562,9 @@
       <c r="E19" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -2575,8 +2580,9 @@
       <c r="E20" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -2592,8 +2598,9 @@
       <c r="E21" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -2609,8 +2616,9 @@
       <c r="E22" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -2626,8 +2634,9 @@
       <c r="E23" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -2643,8 +2652,9 @@
       <c r="E24" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -2660,6 +2670,7 @@
       <c r="E25" s="4" t="s">
         <v>52</v>
       </c>
+      <c r="F25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>